<commit_message>
update 30 11 20
</commit_message>
<xml_diff>
--- a/datos/almendralejo.xlsx
+++ b/datos/almendralejo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharias/Documents/proyectos/covid_almendralejo/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CF9F54C-5C4A-C641-A6EC-8B82ECABE8FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5462D6E-B3A9-BA48-9D98-34BEB8BFD8A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12140" yWindow="-27720" windowWidth="12420" windowHeight="23200" xr2:uid="{48BB2F20-3982-A54D-86CC-9264A1A7C17D}"/>
   </bookViews>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DD655E-19DC-6347-97FE-29D4FEA61905}">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,6 +799,14 @@
         <v>3</v>
       </c>
     </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>44165</v>
+      </c>
+      <c r="B47">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
update 01 12 20
</commit_message>
<xml_diff>
--- a/datos/almendralejo.xlsx
+++ b/datos/almendralejo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mharias/Documents/proyectos/covid_almendralejo/datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F245749-742F-9C46-9726-C4089B81341C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCC60FC6-2108-0640-9026-4ADCB6D31C0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12140" yWindow="-27720" windowWidth="12420" windowHeight="23200" xr2:uid="{48BB2F20-3982-A54D-86CC-9264A1A7C17D}"/>
   </bookViews>
@@ -401,10 +401,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7DD655E-19DC-6347-97FE-29D4FEA61905}">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -807,6 +807,14 @@
         <v>5</v>
       </c>
     </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>44166</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>